<commit_message>
Minimal -> Niveau 7
</commit_message>
<xml_diff>
--- a/Enigma - Prototype.xlsx
+++ b/Enigma - Prototype.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="6" documentId="63E2BC6621E43059836B63AEED78B6F68789A9E6" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{478560D1-487F-4594-BBD5-5615A2C51693}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -586,9 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.85546875" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>